<commit_message>
update tiến độ công việc
</commit_message>
<xml_diff>
--- a/SWP/References/OnlineLearn_Function Details.xlsx
+++ b/SWP/References/OnlineLearn_Function Details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="9072"/>
+    <workbookView windowWidth="23040" windowHeight="9215"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,9 +512,64 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -526,59 +581,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -587,26 +589,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -618,13 +618,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -634,6 +627,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -667,19 +667,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,157 +841,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -866,15 +866,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -918,17 +909,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -944,6 +929,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -970,7 +970,7 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -986,64 +986,64 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1052,65 +1052,65 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1570,9 +1570,9 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16:F49"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="11">
-        <f>ROW()-9</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B31" s="17" t="s">

</xml_diff>